<commit_message>
create and test a few different optimization approaches - adaptive cooling seems to be the only one maybe worth keeping around as it seems add more consistency to the solve time without any cost of slowdown
</commit_message>
<xml_diff>
--- a/docs/resources/Building Layout Speed Testing Data.xlsx
+++ b/docs/resources/Building Layout Speed Testing Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/code/ForceDrawnGraphs/docs/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F3EF42-6B88-BD4B-9F16-4500243B2E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62836FE-32BA-1C46-A032-77A2F0B8305B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{56B1BAED-46F8-334C-B737-A9E8FC8C6838}"/>
   </bookViews>
@@ -19,8 +19,10 @@
     <definedName name="debug" localSheetId="0">'Runs1-3 v1'!$A$2:$A$24</definedName>
     <definedName name="debug_1" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
     <definedName name="debug_2" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
+    <definedName name="debug_3" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
+    <definedName name="debug_4" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +45,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{2E82D927-6DC5-C44C-AC86-E39FAD665377}" name="debug" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/debug.log">
+    <textPr sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/debug.log">
       <textFields>
         <textField/>
       </textFields>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>FRLayout::</t>
   </si>
@@ -65,6 +67,15 @@
   </si>
   <si>
     <t>AVG</t>
+  </si>
+  <si>
+    <t>AdaptiveCooling::</t>
+  </si>
+  <si>
+    <t>DistanceCache::</t>
+  </si>
+  <si>
+    <t>This also requires a distance calculation… Wonder if both would work well together</t>
   </si>
 </sst>
 </file>
@@ -87,18 +98,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -118,6 +123,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -131,23 +154,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20455577-B728-704B-90EB-50FFA7ABC561}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,13 +528,25 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -533,8 +576,32 @@
       <c r="K1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>92</v>
       </c>
@@ -564,8 +631,24 @@
       <c r="K2" s="6">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="R2" s="10">
+        <v>85</v>
+      </c>
+      <c r="S2" s="6">
+        <v>111</v>
+      </c>
+      <c r="T2" s="6">
+        <v>88</v>
+      </c>
+      <c r="U2" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>106</v>
       </c>
@@ -595,8 +678,32 @@
       <c r="K3" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" s="10">
+        <v>93</v>
+      </c>
+      <c r="N3" s="10">
+        <v>79</v>
+      </c>
+      <c r="O3" s="10">
+        <v>114</v>
+      </c>
+      <c r="P3" s="10">
+        <v>88</v>
+      </c>
+      <c r="R3" s="10">
+        <v>88</v>
+      </c>
+      <c r="S3" s="6">
+        <v>84</v>
+      </c>
+      <c r="T3" s="6">
+        <v>92</v>
+      </c>
+      <c r="U3" s="6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>71</v>
       </c>
@@ -626,8 +733,32 @@
       <c r="K4" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" s="10">
+        <v>70</v>
+      </c>
+      <c r="N4" s="10">
+        <v>58</v>
+      </c>
+      <c r="O4" s="10">
+        <v>86</v>
+      </c>
+      <c r="P4" s="10">
+        <v>87</v>
+      </c>
+      <c r="R4" s="10">
+        <v>70</v>
+      </c>
+      <c r="S4" s="6">
+        <v>84</v>
+      </c>
+      <c r="T4" s="6">
+        <v>85</v>
+      </c>
+      <c r="U4" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>70</v>
       </c>
@@ -657,8 +788,32 @@
       <c r="K5" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" s="10">
+        <v>68</v>
+      </c>
+      <c r="N5" s="10">
+        <v>56</v>
+      </c>
+      <c r="O5" s="10">
+        <v>86</v>
+      </c>
+      <c r="P5" s="10">
+        <v>87</v>
+      </c>
+      <c r="R5" s="10">
+        <v>67</v>
+      </c>
+      <c r="S5" s="6">
+        <v>85</v>
+      </c>
+      <c r="T5" s="6">
+        <v>86</v>
+      </c>
+      <c r="U5" s="6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>71</v>
       </c>
@@ -688,8 +843,32 @@
       <c r="K6" s="6">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="10">
+        <v>71</v>
+      </c>
+      <c r="N6" s="10">
+        <v>60</v>
+      </c>
+      <c r="O6" s="10">
+        <v>85</v>
+      </c>
+      <c r="P6" s="10">
+        <v>86</v>
+      </c>
+      <c r="R6" s="10">
+        <v>73</v>
+      </c>
+      <c r="S6" s="6">
+        <v>85</v>
+      </c>
+      <c r="T6" s="6">
+        <v>86</v>
+      </c>
+      <c r="U6" s="6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>71</v>
       </c>
@@ -719,8 +898,32 @@
       <c r="K7" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" s="10">
+        <v>71</v>
+      </c>
+      <c r="N7" s="10">
+        <v>55</v>
+      </c>
+      <c r="O7" s="10">
+        <v>85</v>
+      </c>
+      <c r="P7" s="10">
+        <v>86</v>
+      </c>
+      <c r="R7" s="10">
+        <v>74</v>
+      </c>
+      <c r="S7" s="6">
+        <v>85</v>
+      </c>
+      <c r="T7" s="6">
+        <v>85</v>
+      </c>
+      <c r="U7" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>64</v>
       </c>
@@ -750,8 +953,32 @@
       <c r="K8" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="10">
+        <v>67</v>
+      </c>
+      <c r="N8" s="10">
+        <v>57</v>
+      </c>
+      <c r="O8" s="10">
+        <v>85</v>
+      </c>
+      <c r="P8" s="10">
+        <v>85</v>
+      </c>
+      <c r="R8" s="10">
+        <v>72</v>
+      </c>
+      <c r="S8" s="6">
+        <v>86</v>
+      </c>
+      <c r="T8" s="6">
+        <v>87</v>
+      </c>
+      <c r="U8" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>68</v>
       </c>
@@ -781,8 +1008,32 @@
       <c r="K9" s="6">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="10">
+        <v>56</v>
+      </c>
+      <c r="N9" s="10">
+        <v>55</v>
+      </c>
+      <c r="O9" s="10">
+        <v>113</v>
+      </c>
+      <c r="P9" s="10">
+        <v>86</v>
+      </c>
+      <c r="R9" s="10">
+        <v>72</v>
+      </c>
+      <c r="S9" s="6">
+        <v>85</v>
+      </c>
+      <c r="T9" s="6">
+        <v>84</v>
+      </c>
+      <c r="U9" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>57</v>
       </c>
@@ -812,8 +1063,32 @@
       <c r="K10" s="6">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="10">
+        <v>71</v>
+      </c>
+      <c r="N10" s="10">
+        <v>56</v>
+      </c>
+      <c r="O10" s="10">
+        <v>87</v>
+      </c>
+      <c r="P10" s="10">
+        <v>87</v>
+      </c>
+      <c r="R10" s="10">
+        <v>72</v>
+      </c>
+      <c r="S10" s="6">
+        <v>87</v>
+      </c>
+      <c r="T10" s="6">
+        <v>86</v>
+      </c>
+      <c r="U10" s="6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>72</v>
       </c>
@@ -843,8 +1118,32 @@
       <c r="K11" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" s="10">
+        <v>71</v>
+      </c>
+      <c r="N11" s="10">
+        <v>56</v>
+      </c>
+      <c r="O11" s="10">
+        <v>93</v>
+      </c>
+      <c r="P11" s="10">
+        <v>87</v>
+      </c>
+      <c r="R11" s="10">
+        <v>71</v>
+      </c>
+      <c r="S11" s="6">
+        <v>84</v>
+      </c>
+      <c r="T11" s="6">
+        <v>86</v>
+      </c>
+      <c r="U11" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>71</v>
       </c>
@@ -874,8 +1173,32 @@
       <c r="K12" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="10">
+        <v>71</v>
+      </c>
+      <c r="N12" s="10">
+        <v>56</v>
+      </c>
+      <c r="O12" s="10">
+        <v>86</v>
+      </c>
+      <c r="P12" s="10">
+        <v>86</v>
+      </c>
+      <c r="R12" s="10">
+        <v>73</v>
+      </c>
+      <c r="S12" s="6">
+        <v>84</v>
+      </c>
+      <c r="T12" s="6">
+        <v>85</v>
+      </c>
+      <c r="U12" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>56</v>
       </c>
@@ -905,8 +1228,32 @@
       <c r="K13" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13" s="10">
+        <v>67</v>
+      </c>
+      <c r="N13" s="10">
+        <v>57</v>
+      </c>
+      <c r="O13" s="10">
+        <v>86</v>
+      </c>
+      <c r="P13" s="10">
+        <v>88</v>
+      </c>
+      <c r="R13" s="10">
+        <v>72</v>
+      </c>
+      <c r="S13" s="6">
+        <v>84</v>
+      </c>
+      <c r="T13" s="6">
+        <v>85</v>
+      </c>
+      <c r="U13" s="6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>80</v>
       </c>
@@ -936,8 +1283,32 @@
       <c r="K14" s="6">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14" s="10">
+        <v>70</v>
+      </c>
+      <c r="N14" s="10">
+        <v>56</v>
+      </c>
+      <c r="O14" s="10">
+        <v>87</v>
+      </c>
+      <c r="P14" s="10">
+        <v>87</v>
+      </c>
+      <c r="R14" s="10">
+        <v>72</v>
+      </c>
+      <c r="S14" s="6">
+        <v>84</v>
+      </c>
+      <c r="T14" s="6">
+        <v>84</v>
+      </c>
+      <c r="U14" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>63</v>
       </c>
@@ -967,8 +1338,32 @@
       <c r="K15" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M15" s="10">
+        <v>70</v>
+      </c>
+      <c r="N15" s="10">
+        <v>56</v>
+      </c>
+      <c r="O15" s="10">
+        <v>86</v>
+      </c>
+      <c r="P15" s="10">
+        <v>87</v>
+      </c>
+      <c r="R15" s="10">
+        <v>72</v>
+      </c>
+      <c r="S15" s="6">
+        <v>84</v>
+      </c>
+      <c r="T15" s="6">
+        <v>84</v>
+      </c>
+      <c r="U15" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>65</v>
       </c>
@@ -998,8 +1393,32 @@
       <c r="K16" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" s="10">
+        <v>65</v>
+      </c>
+      <c r="N16" s="10">
+        <v>56</v>
+      </c>
+      <c r="O16" s="10">
+        <v>86</v>
+      </c>
+      <c r="P16" s="10">
+        <v>87</v>
+      </c>
+      <c r="R16" s="10">
+        <v>69</v>
+      </c>
+      <c r="S16" s="6">
+        <v>84</v>
+      </c>
+      <c r="T16" s="6">
+        <v>87</v>
+      </c>
+      <c r="U16" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>62</v>
       </c>
@@ -1029,8 +1448,32 @@
       <c r="K17" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17" s="10">
+        <v>72</v>
+      </c>
+      <c r="N17" s="10">
+        <v>56</v>
+      </c>
+      <c r="O17" s="10">
+        <v>86</v>
+      </c>
+      <c r="P17" s="10">
+        <v>90</v>
+      </c>
+      <c r="R17" s="10">
+        <v>72</v>
+      </c>
+      <c r="S17" s="6">
+        <v>85</v>
+      </c>
+      <c r="T17" s="6">
+        <v>86</v>
+      </c>
+      <c r="U17" s="6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>70</v>
       </c>
@@ -1060,8 +1503,32 @@
       <c r="K18" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="10">
+        <v>68</v>
+      </c>
+      <c r="N18" s="10">
+        <v>57</v>
+      </c>
+      <c r="O18" s="10">
+        <v>85</v>
+      </c>
+      <c r="P18" s="10">
+        <v>85</v>
+      </c>
+      <c r="R18" s="10">
+        <v>73</v>
+      </c>
+      <c r="S18" s="6">
+        <v>87</v>
+      </c>
+      <c r="T18" s="6">
+        <v>90</v>
+      </c>
+      <c r="U18" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>65</v>
       </c>
@@ -1091,8 +1558,32 @@
       <c r="K19" s="6">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19" s="10">
+        <v>73</v>
+      </c>
+      <c r="N19" s="10">
+        <v>55</v>
+      </c>
+      <c r="O19" s="10">
+        <v>85</v>
+      </c>
+      <c r="P19" s="10">
+        <v>86</v>
+      </c>
+      <c r="R19" s="10">
+        <v>74</v>
+      </c>
+      <c r="S19" s="6">
+        <v>85</v>
+      </c>
+      <c r="T19" s="6">
+        <v>87</v>
+      </c>
+      <c r="U19" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>71</v>
       </c>
@@ -1122,8 +1613,32 @@
       <c r="K20" s="6">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" s="10">
+        <v>70</v>
+      </c>
+      <c r="N20" s="10">
+        <v>57</v>
+      </c>
+      <c r="O20" s="10">
+        <v>85</v>
+      </c>
+      <c r="P20" s="10">
+        <v>86</v>
+      </c>
+      <c r="R20" s="10">
+        <v>69</v>
+      </c>
+      <c r="S20" s="6">
+        <v>87</v>
+      </c>
+      <c r="T20" s="6">
+        <v>84</v>
+      </c>
+      <c r="U20" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>57</v>
       </c>
@@ -1153,8 +1668,32 @@
       <c r="K21" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21" s="10">
+        <v>71</v>
+      </c>
+      <c r="N21" s="10">
+        <v>56</v>
+      </c>
+      <c r="O21" s="10">
+        <v>112</v>
+      </c>
+      <c r="P21" s="10">
+        <v>85</v>
+      </c>
+      <c r="R21" s="10">
+        <v>75</v>
+      </c>
+      <c r="S21" s="6">
+        <v>86</v>
+      </c>
+      <c r="T21" s="6">
+        <v>85</v>
+      </c>
+      <c r="U21" s="6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>69</v>
       </c>
@@ -1165,9 +1704,9 @@
         <v>85</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="5"/>
       <c r="I22" s="6">
         <v>66</v>
@@ -1178,8 +1717,24 @@
       <c r="K22" s="6">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="R22" s="10">
+        <v>57</v>
+      </c>
+      <c r="S22" s="6">
+        <v>85</v>
+      </c>
+      <c r="T22" s="6">
+        <v>85</v>
+      </c>
+      <c r="U22" s="6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f>AVERAGE(A2:A22)</f>
         <v>70.047619047619051</v>
@@ -1221,6 +1776,145 @@
       <c r="K23" s="4">
         <f>AVERAGE(K2:K22)</f>
         <v>85.61904761904762</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" s="2">
+        <f>AVERAGE(M3:M21)</f>
+        <v>70.263157894736835</v>
+      </c>
+      <c r="N23" s="3">
+        <f>AVERAGE(N3:N21)</f>
+        <v>57.578947368421055</v>
+      </c>
+      <c r="O23" s="4">
+        <f>AVERAGE(O3:O21)</f>
+        <v>90.421052631578945</v>
+      </c>
+      <c r="P23" s="12">
+        <f>AVERAGE(P3:P21)</f>
+        <v>86.631578947368425</v>
+      </c>
+      <c r="R23" s="10">
+        <v>72</v>
+      </c>
+      <c r="S23" s="6">
+        <v>84</v>
+      </c>
+      <c r="T23" s="6">
+        <v>85</v>
+      </c>
+      <c r="U23" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R24" s="10">
+        <v>72</v>
+      </c>
+      <c r="S24" s="6">
+        <v>85</v>
+      </c>
+      <c r="T24" s="6">
+        <v>85</v>
+      </c>
+      <c r="U24" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R25" s="10">
+        <v>71</v>
+      </c>
+      <c r="S25" s="6">
+        <v>85</v>
+      </c>
+      <c r="T25" s="6">
+        <v>85</v>
+      </c>
+      <c r="U25" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R26" s="10">
+        <v>73</v>
+      </c>
+      <c r="S26" s="6">
+        <v>85</v>
+      </c>
+      <c r="T26" s="6">
+        <v>85</v>
+      </c>
+      <c r="U26" s="6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R27" s="10">
+        <v>66</v>
+      </c>
+      <c r="S27" s="6">
+        <v>86</v>
+      </c>
+      <c r="T27" s="6">
+        <v>85</v>
+      </c>
+      <c r="U27" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R28" s="10">
+        <v>72</v>
+      </c>
+      <c r="S28" s="6">
+        <v>85</v>
+      </c>
+      <c r="T28" s="6">
+        <v>115</v>
+      </c>
+      <c r="U28" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P29" s="8"/>
+      <c r="R29" s="10">
+        <v>59</v>
+      </c>
+      <c r="S29" s="6">
+        <v>88</v>
+      </c>
+      <c r="T29" s="6">
+        <v>88</v>
+      </c>
+      <c r="U29" s="6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R30" s="3">
+        <f>AVERAGE(R2:R29)</f>
+        <v>71.678571428571431</v>
+      </c>
+      <c r="S30" s="4">
+        <f>AVERAGE(S2:S29)</f>
+        <v>86.035714285714292</v>
+      </c>
+      <c r="T30" s="12">
+        <f>AVERAGE(T2:T29)</f>
+        <v>86.964285714285708</v>
+      </c>
+      <c r="U30" s="13">
+        <f>AVERAGE(U2:U29)</f>
+        <v>136.32142857142858</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continued testing on adaptive and not
</commit_message>
<xml_diff>
--- a/docs/resources/Building Layout Speed Testing Data.xlsx
+++ b/docs/resources/Building Layout Speed Testing Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/code/ForceDrawnGraphs/docs/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62836FE-32BA-1C46-A032-77A2F0B8305B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4706FF31-A416-3F44-B05F-7DFCE72DB200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{56B1BAED-46F8-334C-B737-A9E8FC8C6838}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="debug_2" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
     <definedName name="debug_3" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
     <definedName name="debug_4" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
+    <definedName name="debug_5" localSheetId="0">'Runs1-3 v1'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
   <si>
     <t>FRLayout::</t>
   </si>
@@ -75,14 +76,20 @@
     <t>DistanceCache::</t>
   </si>
   <si>
-    <t>This also requires a distance calculation… Wonder if both would work well together</t>
+    <t>FRLayout3D:</t>
+  </si>
+  <si>
+    <t>AdaptiveCooling:</t>
+  </si>
+  <si>
+    <t>Cumulative Averages:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,8 +104,16 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +156,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -171,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -179,6 +201,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20455577-B728-704B-90EB-50FFA7ABC561}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,13 +565,19 @@
     <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -600,8 +631,20 @@
       <c r="U1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>92</v>
       </c>
@@ -635,7 +678,7 @@
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
-      <c r="R2" s="10">
+      <c r="R2" s="11">
         <v>85</v>
       </c>
       <c r="S2" s="6">
@@ -647,8 +690,20 @@
       <c r="U2" s="6">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W2" s="6">
+        <v>94</v>
+      </c>
+      <c r="X2" s="6">
+        <v>80</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>115</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>106</v>
       </c>
@@ -678,19 +733,19 @@
       <c r="K3" s="6">
         <v>85</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="11">
         <v>93</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="11">
         <v>79</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="11">
         <v>114</v>
       </c>
-      <c r="P3" s="10">
-        <v>88</v>
-      </c>
-      <c r="R3" s="10">
+      <c r="P3" s="11">
+        <v>88</v>
+      </c>
+      <c r="R3" s="11">
         <v>88</v>
       </c>
       <c r="S3" s="6">
@@ -702,8 +757,21 @@
       <c r="U3" s="6">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W3" s="6">
+        <v>104</v>
+      </c>
+      <c r="X3" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="10"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>71</v>
       </c>
@@ -733,19 +801,19 @@
       <c r="K4" s="6">
         <v>85</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="11">
         <v>70</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="11">
         <v>58</v>
       </c>
-      <c r="O4" s="10">
-        <v>86</v>
-      </c>
-      <c r="P4" s="10">
-        <v>87</v>
-      </c>
-      <c r="R4" s="10">
+      <c r="O4" s="11">
+        <v>86</v>
+      </c>
+      <c r="P4" s="11">
+        <v>87</v>
+      </c>
+      <c r="R4" s="11">
         <v>70</v>
       </c>
       <c r="S4" s="6">
@@ -757,8 +825,21 @@
       <c r="U4" s="6">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W4" s="6">
+        <v>73</v>
+      </c>
+      <c r="X4" s="6">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>89</v>
+      </c>
+      <c r="AC4" s="10"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>70</v>
       </c>
@@ -788,19 +869,19 @@
       <c r="K5" s="6">
         <v>83</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="11">
         <v>68</v>
       </c>
-      <c r="N5" s="10">
-        <v>56</v>
-      </c>
-      <c r="O5" s="10">
-        <v>86</v>
-      </c>
-      <c r="P5" s="10">
-        <v>87</v>
-      </c>
-      <c r="R5" s="10">
+      <c r="N5" s="11">
+        <v>56</v>
+      </c>
+      <c r="O5" s="11">
+        <v>86</v>
+      </c>
+      <c r="P5" s="11">
+        <v>87</v>
+      </c>
+      <c r="R5" s="11">
         <v>67</v>
       </c>
       <c r="S5" s="6">
@@ -812,8 +893,20 @@
       <c r="U5" s="6">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W5" s="6">
+        <v>72</v>
+      </c>
+      <c r="X5" s="6">
+        <v>62</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>71</v>
       </c>
@@ -843,19 +936,19 @@
       <c r="K6" s="6">
         <v>84</v>
       </c>
-      <c r="M6" s="10">
-        <v>71</v>
-      </c>
-      <c r="N6" s="10">
+      <c r="M6" s="11">
+        <v>71</v>
+      </c>
+      <c r="N6" s="11">
         <v>60</v>
       </c>
-      <c r="O6" s="10">
-        <v>85</v>
-      </c>
-      <c r="P6" s="10">
-        <v>86</v>
-      </c>
-      <c r="R6" s="10">
+      <c r="O6" s="11">
+        <v>85</v>
+      </c>
+      <c r="P6" s="11">
+        <v>86</v>
+      </c>
+      <c r="R6" s="11">
         <v>73</v>
       </c>
       <c r="S6" s="6">
@@ -867,8 +960,20 @@
       <c r="U6" s="6">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W6" s="6">
+        <v>73</v>
+      </c>
+      <c r="X6" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>71</v>
       </c>
@@ -898,19 +1003,19 @@
       <c r="K7" s="6">
         <v>83</v>
       </c>
-      <c r="M7" s="10">
-        <v>71</v>
-      </c>
-      <c r="N7" s="10">
+      <c r="M7" s="11">
+        <v>71</v>
+      </c>
+      <c r="N7" s="11">
         <v>55</v>
       </c>
-      <c r="O7" s="10">
-        <v>85</v>
-      </c>
-      <c r="P7" s="10">
-        <v>86</v>
-      </c>
-      <c r="R7" s="10">
+      <c r="O7" s="11">
+        <v>85</v>
+      </c>
+      <c r="P7" s="11">
+        <v>86</v>
+      </c>
+      <c r="R7" s="11">
         <v>74</v>
       </c>
       <c r="S7" s="6">
@@ -922,8 +1027,20 @@
       <c r="U7" s="6">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W7" s="6">
+        <v>64</v>
+      </c>
+      <c r="X7" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>64</v>
       </c>
@@ -953,19 +1070,19 @@
       <c r="K8" s="6">
         <v>83</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="11">
         <v>67</v>
       </c>
-      <c r="N8" s="10">
-        <v>57</v>
-      </c>
-      <c r="O8" s="10">
-        <v>85</v>
-      </c>
-      <c r="P8" s="10">
-        <v>85</v>
-      </c>
-      <c r="R8" s="10">
+      <c r="N8" s="11">
+        <v>57</v>
+      </c>
+      <c r="O8" s="11">
+        <v>85</v>
+      </c>
+      <c r="P8" s="11">
+        <v>85</v>
+      </c>
+      <c r="R8" s="11">
         <v>72</v>
       </c>
       <c r="S8" s="6">
@@ -977,8 +1094,20 @@
       <c r="U8" s="6">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W8" s="6">
+        <v>73</v>
+      </c>
+      <c r="X8" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y8" s="6">
+        <v>89</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>68</v>
       </c>
@@ -1008,19 +1137,19 @@
       <c r="K9" s="6">
         <v>85</v>
       </c>
-      <c r="M9" s="10">
-        <v>56</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="M9" s="11">
+        <v>56</v>
+      </c>
+      <c r="N9" s="11">
         <v>55</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="11">
         <v>113</v>
       </c>
-      <c r="P9" s="10">
-        <v>86</v>
-      </c>
-      <c r="R9" s="10">
+      <c r="P9" s="11">
+        <v>86</v>
+      </c>
+      <c r="R9" s="11">
         <v>72</v>
       </c>
       <c r="S9" s="6">
@@ -1032,8 +1161,20 @@
       <c r="U9" s="6">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W9" s="6">
+        <v>70</v>
+      </c>
+      <c r="X9" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>57</v>
       </c>
@@ -1063,19 +1204,19 @@
       <c r="K10" s="6">
         <v>82</v>
       </c>
-      <c r="M10" s="10">
-        <v>71</v>
-      </c>
-      <c r="N10" s="10">
-        <v>56</v>
-      </c>
-      <c r="O10" s="10">
-        <v>87</v>
-      </c>
-      <c r="P10" s="10">
-        <v>87</v>
-      </c>
-      <c r="R10" s="10">
+      <c r="M10" s="11">
+        <v>71</v>
+      </c>
+      <c r="N10" s="11">
+        <v>56</v>
+      </c>
+      <c r="O10" s="11">
+        <v>87</v>
+      </c>
+      <c r="P10" s="11">
+        <v>87</v>
+      </c>
+      <c r="R10" s="11">
         <v>72</v>
       </c>
       <c r="S10" s="6">
@@ -1087,8 +1228,20 @@
       <c r="U10" s="6">
         <v>138</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W10" s="6">
+        <v>72</v>
+      </c>
+      <c r="X10" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>95</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>72</v>
       </c>
@@ -1118,19 +1271,19 @@
       <c r="K11" s="6">
         <v>83</v>
       </c>
-      <c r="M11" s="10">
-        <v>71</v>
-      </c>
-      <c r="N11" s="10">
-        <v>56</v>
-      </c>
-      <c r="O11" s="10">
+      <c r="M11" s="11">
+        <v>71</v>
+      </c>
+      <c r="N11" s="11">
+        <v>56</v>
+      </c>
+      <c r="O11" s="11">
         <v>93</v>
       </c>
-      <c r="P11" s="10">
-        <v>87</v>
-      </c>
-      <c r="R11" s="10">
+      <c r="P11" s="11">
+        <v>87</v>
+      </c>
+      <c r="R11" s="11">
         <v>71</v>
       </c>
       <c r="S11" s="6">
@@ -1142,8 +1295,20 @@
       <c r="U11" s="6">
         <v>135</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W11" s="6">
+        <v>73</v>
+      </c>
+      <c r="X11" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>71</v>
       </c>
@@ -1173,19 +1338,19 @@
       <c r="K12" s="6">
         <v>83</v>
       </c>
-      <c r="M12" s="10">
-        <v>71</v>
-      </c>
-      <c r="N12" s="10">
-        <v>56</v>
-      </c>
-      <c r="O12" s="10">
-        <v>86</v>
-      </c>
-      <c r="P12" s="10">
-        <v>86</v>
-      </c>
-      <c r="R12" s="10">
+      <c r="M12" s="11">
+        <v>71</v>
+      </c>
+      <c r="N12" s="11">
+        <v>56</v>
+      </c>
+      <c r="O12" s="11">
+        <v>86</v>
+      </c>
+      <c r="P12" s="11">
+        <v>86</v>
+      </c>
+      <c r="R12" s="11">
         <v>73</v>
       </c>
       <c r="S12" s="6">
@@ -1197,8 +1362,20 @@
       <c r="U12" s="6">
         <v>135</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W12" s="6">
+        <v>72</v>
+      </c>
+      <c r="X12" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>56</v>
       </c>
@@ -1228,19 +1405,19 @@
       <c r="K13" s="6">
         <v>83</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="11">
         <v>67</v>
       </c>
-      <c r="N13" s="10">
-        <v>57</v>
-      </c>
-      <c r="O13" s="10">
-        <v>86</v>
-      </c>
-      <c r="P13" s="10">
-        <v>88</v>
-      </c>
-      <c r="R13" s="10">
+      <c r="N13" s="11">
+        <v>57</v>
+      </c>
+      <c r="O13" s="11">
+        <v>86</v>
+      </c>
+      <c r="P13" s="11">
+        <v>88</v>
+      </c>
+      <c r="R13" s="11">
         <v>72</v>
       </c>
       <c r="S13" s="6">
@@ -1252,8 +1429,20 @@
       <c r="U13" s="6">
         <v>143</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W13" s="6">
+        <v>73</v>
+      </c>
+      <c r="X13" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>80</v>
       </c>
@@ -1283,19 +1472,19 @@
       <c r="K14" s="6">
         <v>82</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="11">
         <v>70</v>
       </c>
-      <c r="N14" s="10">
-        <v>56</v>
-      </c>
-      <c r="O14" s="10">
-        <v>87</v>
-      </c>
-      <c r="P14" s="10">
-        <v>87</v>
-      </c>
-      <c r="R14" s="10">
+      <c r="N14" s="11">
+        <v>56</v>
+      </c>
+      <c r="O14" s="11">
+        <v>87</v>
+      </c>
+      <c r="P14" s="11">
+        <v>87</v>
+      </c>
+      <c r="R14" s="11">
         <v>72</v>
       </c>
       <c r="S14" s="6">
@@ -1307,8 +1496,20 @@
       <c r="U14" s="6">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W14" s="6">
+        <v>60</v>
+      </c>
+      <c r="X14" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>63</v>
       </c>
@@ -1338,19 +1539,19 @@
       <c r="K15" s="6">
         <v>83</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="11">
         <v>70</v>
       </c>
-      <c r="N15" s="10">
-        <v>56</v>
-      </c>
-      <c r="O15" s="10">
-        <v>86</v>
-      </c>
-      <c r="P15" s="10">
-        <v>87</v>
-      </c>
-      <c r="R15" s="10">
+      <c r="N15" s="11">
+        <v>56</v>
+      </c>
+      <c r="O15" s="11">
+        <v>86</v>
+      </c>
+      <c r="P15" s="11">
+        <v>87</v>
+      </c>
+      <c r="R15" s="11">
         <v>72</v>
       </c>
       <c r="S15" s="6">
@@ -1362,8 +1563,20 @@
       <c r="U15" s="6">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W15" s="6">
+        <v>71</v>
+      </c>
+      <c r="X15" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>65</v>
       </c>
@@ -1393,19 +1606,19 @@
       <c r="K16" s="6">
         <v>83</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="11">
         <v>65</v>
       </c>
-      <c r="N16" s="10">
-        <v>56</v>
-      </c>
-      <c r="O16" s="10">
-        <v>86</v>
-      </c>
-      <c r="P16" s="10">
-        <v>87</v>
-      </c>
-      <c r="R16" s="10">
+      <c r="N16" s="11">
+        <v>56</v>
+      </c>
+      <c r="O16" s="11">
+        <v>86</v>
+      </c>
+      <c r="P16" s="11">
+        <v>87</v>
+      </c>
+      <c r="R16" s="11">
         <v>69</v>
       </c>
       <c r="S16" s="6">
@@ -1417,8 +1630,20 @@
       <c r="U16" s="6">
         <v>131</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W16" s="6">
+        <v>72</v>
+      </c>
+      <c r="X16" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>89</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>62</v>
       </c>
@@ -1448,19 +1673,19 @@
       <c r="K17" s="6">
         <v>83</v>
       </c>
-      <c r="M17" s="10">
-        <v>72</v>
-      </c>
-      <c r="N17" s="10">
-        <v>56</v>
-      </c>
-      <c r="O17" s="10">
-        <v>86</v>
-      </c>
-      <c r="P17" s="10">
+      <c r="M17" s="11">
+        <v>72</v>
+      </c>
+      <c r="N17" s="11">
+        <v>56</v>
+      </c>
+      <c r="O17" s="11">
+        <v>86</v>
+      </c>
+      <c r="P17" s="11">
         <v>90</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="11">
         <v>72</v>
       </c>
       <c r="S17" s="6">
@@ -1472,8 +1697,20 @@
       <c r="U17" s="6">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W17" s="6">
+        <v>72</v>
+      </c>
+      <c r="X17" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y17" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z17" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>70</v>
       </c>
@@ -1503,19 +1740,19 @@
       <c r="K18" s="6">
         <v>83</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="11">
         <v>68</v>
       </c>
-      <c r="N18" s="10">
-        <v>57</v>
-      </c>
-      <c r="O18" s="10">
-        <v>85</v>
-      </c>
-      <c r="P18" s="10">
-        <v>85</v>
-      </c>
-      <c r="R18" s="10">
+      <c r="N18" s="11">
+        <v>57</v>
+      </c>
+      <c r="O18" s="11">
+        <v>85</v>
+      </c>
+      <c r="P18" s="11">
+        <v>85</v>
+      </c>
+      <c r="R18" s="11">
         <v>73</v>
       </c>
       <c r="S18" s="6">
@@ -1527,8 +1764,20 @@
       <c r="U18" s="6">
         <v>133</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W18" s="6">
+        <v>70</v>
+      </c>
+      <c r="X18" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z18" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>65</v>
       </c>
@@ -1558,19 +1807,19 @@
       <c r="K19" s="6">
         <v>104</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="11">
         <v>73</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="11">
         <v>55</v>
       </c>
-      <c r="O19" s="10">
-        <v>85</v>
-      </c>
-      <c r="P19" s="10">
-        <v>86</v>
-      </c>
-      <c r="R19" s="10">
+      <c r="O19" s="11">
+        <v>85</v>
+      </c>
+      <c r="P19" s="11">
+        <v>86</v>
+      </c>
+      <c r="R19" s="11">
         <v>74</v>
       </c>
       <c r="S19" s="6">
@@ -1582,8 +1831,20 @@
       <c r="U19" s="6">
         <v>134</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W19" s="6">
+        <v>73</v>
+      </c>
+      <c r="X19" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y19" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z19" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>71</v>
       </c>
@@ -1613,19 +1874,19 @@
       <c r="K20" s="6">
         <v>82</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="11">
         <v>70</v>
       </c>
-      <c r="N20" s="10">
-        <v>57</v>
-      </c>
-      <c r="O20" s="10">
-        <v>85</v>
-      </c>
-      <c r="P20" s="10">
-        <v>86</v>
-      </c>
-      <c r="R20" s="10">
+      <c r="N20" s="11">
+        <v>57</v>
+      </c>
+      <c r="O20" s="11">
+        <v>85</v>
+      </c>
+      <c r="P20" s="11">
+        <v>86</v>
+      </c>
+      <c r="R20" s="11">
         <v>69</v>
       </c>
       <c r="S20" s="6">
@@ -1637,8 +1898,20 @@
       <c r="U20" s="6">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W20" s="6">
+        <v>73</v>
+      </c>
+      <c r="X20" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y20" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z20" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>57</v>
       </c>
@@ -1668,19 +1941,19 @@
       <c r="K21" s="6">
         <v>83</v>
       </c>
-      <c r="M21" s="10">
-        <v>71</v>
-      </c>
-      <c r="N21" s="10">
-        <v>56</v>
-      </c>
-      <c r="O21" s="10">
+      <c r="M21" s="11">
+        <v>71</v>
+      </c>
+      <c r="N21" s="11">
+        <v>56</v>
+      </c>
+      <c r="O21" s="11">
         <v>112</v>
       </c>
-      <c r="P21" s="10">
-        <v>85</v>
-      </c>
-      <c r="R21" s="10">
+      <c r="P21" s="11">
+        <v>85</v>
+      </c>
+      <c r="R21" s="11">
         <v>75</v>
       </c>
       <c r="S21" s="6">
@@ -1692,8 +1965,20 @@
       <c r="U21" s="6">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W21" s="6">
+        <v>72</v>
+      </c>
+      <c r="X21" s="6">
+        <v>59</v>
+      </c>
+      <c r="Y21" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z21" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>69</v>
       </c>
@@ -1704,9 +1989,9 @@
         <v>85</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="5"/>
       <c r="I22" s="6">
         <v>66</v>
@@ -1721,7 +2006,7 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
-      <c r="R22" s="10">
+      <c r="R22" s="11">
         <v>57</v>
       </c>
       <c r="S22" s="6">
@@ -1733,8 +2018,20 @@
       <c r="U22" s="6">
         <v>164</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W22" s="6">
+        <v>72</v>
+      </c>
+      <c r="X22" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y22" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z22" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f>AVERAGE(A2:A22)</f>
         <v>70.047619047619051</v>
@@ -1792,11 +2089,14 @@
         <f>AVERAGE(O3:O21)</f>
         <v>90.421052631578945</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="13">
         <f>AVERAGE(P3:P21)</f>
         <v>86.631578947368425</v>
       </c>
-      <c r="R23" s="10">
+      <c r="Q23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="11">
         <v>72</v>
       </c>
       <c r="S23" s="6">
@@ -1808,9 +2108,21 @@
       <c r="U23" s="6">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R24" s="10">
+      <c r="W23" s="6">
+        <v>76</v>
+      </c>
+      <c r="X23" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y23" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z23" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R24" s="11">
         <v>72</v>
       </c>
       <c r="S24" s="6">
@@ -1822,9 +2134,21 @@
       <c r="U24" s="6">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R25" s="10">
+      <c r="W24" s="6">
+        <v>60</v>
+      </c>
+      <c r="X24" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y24" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z24" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R25" s="11">
         <v>71</v>
       </c>
       <c r="S25" s="6">
@@ -1836,9 +2160,21 @@
       <c r="U25" s="6">
         <v>133</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R26" s="10">
+      <c r="W25" s="6">
+        <v>65</v>
+      </c>
+      <c r="X25" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y25" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z25" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R26" s="11">
         <v>73</v>
       </c>
       <c r="S26" s="6">
@@ -1850,9 +2186,21 @@
       <c r="U26" s="6">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R27" s="10">
+      <c r="W26" s="6">
+        <v>76</v>
+      </c>
+      <c r="X26" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y26" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z26" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R27" s="11">
         <v>66</v>
       </c>
       <c r="S27" s="6">
@@ -1864,9 +2212,21 @@
       <c r="U27" s="6">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R28" s="10">
+      <c r="W27" s="6">
+        <v>71</v>
+      </c>
+      <c r="X27" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z27" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R28" s="11">
         <v>72</v>
       </c>
       <c r="S28" s="6">
@@ -1878,10 +2238,22 @@
       <c r="U28" s="6">
         <v>133</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W28" s="6">
+        <v>72</v>
+      </c>
+      <c r="X28" s="6">
+        <v>56</v>
+      </c>
+      <c r="Y28" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z28" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="P29" s="8"/>
-      <c r="R29" s="10">
+      <c r="R29" s="11">
         <v>59</v>
       </c>
       <c r="S29" s="6">
@@ -1893,8 +2265,23 @@
       <c r="U29" s="6">
         <v>137</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W29" s="6">
+        <v>73</v>
+      </c>
+      <c r="X29" s="6">
+        <v>61</v>
+      </c>
+      <c r="Y29" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z29" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Q30" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="R30" s="3">
         <f>AVERAGE(R2:R29)</f>
         <v>71.678571428571431</v>
@@ -1903,18 +2290,150 @@
         <f>AVERAGE(S2:S29)</f>
         <v>86.035714285714292</v>
       </c>
-      <c r="T30" s="12">
+      <c r="T30" s="13">
         <f>AVERAGE(T2:T29)</f>
         <v>86.964285714285708</v>
       </c>
-      <c r="U30" s="13">
+      <c r="U30" s="14">
         <f>AVERAGE(U2:U29)</f>
         <v>136.32142857142858</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T31" t="s">
+      <c r="V30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W30" s="6">
+        <v>68</v>
+      </c>
+      <c r="X30" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y30" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z30" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="W31" s="6">
+        <v>72</v>
+      </c>
+      <c r="X31" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y31" s="6">
+        <v>88</v>
+      </c>
+      <c r="Z31" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="W32" s="6">
+        <v>71</v>
+      </c>
+      <c r="X32" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y32" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z32" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="W33" s="6">
+        <v>109</v>
+      </c>
+      <c r="X33" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y33" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z33" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="W34" s="6">
+        <v>71</v>
+      </c>
+      <c r="X34" s="6">
+        <v>58</v>
+      </c>
+      <c r="Y34" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z34" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="R35" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="W35" s="6">
+        <v>71</v>
+      </c>
+      <c r="X35" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y35" s="6">
+        <v>91</v>
+      </c>
+      <c r="Z35" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="R36" s="15" t="s">
         <v>6</v>
+      </c>
+      <c r="S36" s="16">
+        <f>AVERAGE(G2:G21,K2:K22,O3:O21,S2:S29,Y2:Y36)</f>
+        <v>87.731707317073173</v>
+      </c>
+      <c r="W36" s="6">
+        <v>72</v>
+      </c>
+      <c r="X36" s="6">
+        <v>57</v>
+      </c>
+      <c r="Y36" s="6">
+        <v>87</v>
+      </c>
+      <c r="Z36" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="R37" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="16">
+        <f>AVERAGE(P3:P21,T2:T29,Z2:Z36)</f>
+        <v>87.792682926829272</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W37" s="2">
+        <f>AVERAGE(W2:W36)</f>
+        <v>73.571428571428569</v>
+      </c>
+      <c r="X37" s="3">
+        <f>AVERAGE(X2:X36)</f>
+        <v>58.285714285714285</v>
+      </c>
+      <c r="Y37" s="4">
+        <f>AVERAGE(Y2:Y36)</f>
+        <v>88.628571428571433</v>
+      </c>
+      <c r="Z37" s="13">
+        <f>AVERAGE(Z2:Z36)</f>
+        <v>89.085714285714289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating docs to include some more final steps, language changes and re-read understanding tweaks
</commit_message>
<xml_diff>
--- a/docs/resources/Building Layout Speed Testing Data.xlsx
+++ b/docs/resources/Building Layout Speed Testing Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/code/ForceDrawnGraphs/docs/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4706FF31-A416-3F44-B05F-7DFCE72DB200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7503EC7A-BCED-8A4E-A2D0-D77230547B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{56B1BAED-46F8-334C-B737-A9E8FC8C6838}"/>
   </bookViews>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,12 +190,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -544,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20455577-B728-704B-90EB-50FFA7ABC561}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +674,7 @@
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
-      <c r="R2" s="11">
+      <c r="R2" s="6">
         <v>85</v>
       </c>
       <c r="S2" s="6">
@@ -733,19 +729,19 @@
       <c r="K3" s="6">
         <v>85</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="6">
         <v>93</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="6">
         <v>79</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="6">
         <v>114</v>
       </c>
-      <c r="P3" s="11">
-        <v>88</v>
-      </c>
-      <c r="R3" s="11">
+      <c r="P3" s="6">
+        <v>88</v>
+      </c>
+      <c r="R3" s="6">
         <v>88</v>
       </c>
       <c r="S3" s="6">
@@ -769,7 +765,7 @@
       <c r="Z3" s="6">
         <v>90</v>
       </c>
-      <c r="AC3" s="10"/>
+      <c r="AC3" s="9"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
@@ -801,19 +797,19 @@
       <c r="K4" s="6">
         <v>85</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="6">
         <v>70</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="6">
         <v>58</v>
       </c>
-      <c r="O4" s="11">
-        <v>86</v>
-      </c>
-      <c r="P4" s="11">
-        <v>87</v>
-      </c>
-      <c r="R4" s="11">
+      <c r="O4" s="6">
+        <v>86</v>
+      </c>
+      <c r="P4" s="6">
+        <v>87</v>
+      </c>
+      <c r="R4" s="6">
         <v>70</v>
       </c>
       <c r="S4" s="6">
@@ -837,7 +833,7 @@
       <c r="Z4" s="6">
         <v>89</v>
       </c>
-      <c r="AC4" s="10"/>
+      <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -869,19 +865,19 @@
       <c r="K5" s="6">
         <v>83</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="6">
         <v>68</v>
       </c>
-      <c r="N5" s="11">
-        <v>56</v>
-      </c>
-      <c r="O5" s="11">
-        <v>86</v>
-      </c>
-      <c r="P5" s="11">
-        <v>87</v>
-      </c>
-      <c r="R5" s="11">
+      <c r="N5" s="6">
+        <v>56</v>
+      </c>
+      <c r="O5" s="6">
+        <v>86</v>
+      </c>
+      <c r="P5" s="6">
+        <v>87</v>
+      </c>
+      <c r="R5" s="6">
         <v>67</v>
       </c>
       <c r="S5" s="6">
@@ -936,19 +932,19 @@
       <c r="K6" s="6">
         <v>84</v>
       </c>
-      <c r="M6" s="11">
-        <v>71</v>
-      </c>
-      <c r="N6" s="11">
+      <c r="M6" s="6">
+        <v>71</v>
+      </c>
+      <c r="N6" s="6">
         <v>60</v>
       </c>
-      <c r="O6" s="11">
-        <v>85</v>
-      </c>
-      <c r="P6" s="11">
-        <v>86</v>
-      </c>
-      <c r="R6" s="11">
+      <c r="O6" s="6">
+        <v>85</v>
+      </c>
+      <c r="P6" s="6">
+        <v>86</v>
+      </c>
+      <c r="R6" s="6">
         <v>73</v>
       </c>
       <c r="S6" s="6">
@@ -1003,19 +999,19 @@
       <c r="K7" s="6">
         <v>83</v>
       </c>
-      <c r="M7" s="11">
-        <v>71</v>
-      </c>
-      <c r="N7" s="11">
+      <c r="M7" s="6">
+        <v>71</v>
+      </c>
+      <c r="N7" s="6">
         <v>55</v>
       </c>
-      <c r="O7" s="11">
-        <v>85</v>
-      </c>
-      <c r="P7" s="11">
-        <v>86</v>
-      </c>
-      <c r="R7" s="11">
+      <c r="O7" s="6">
+        <v>85</v>
+      </c>
+      <c r="P7" s="6">
+        <v>86</v>
+      </c>
+      <c r="R7" s="6">
         <v>74</v>
       </c>
       <c r="S7" s="6">
@@ -1070,19 +1066,19 @@
       <c r="K8" s="6">
         <v>83</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="6">
         <v>67</v>
       </c>
-      <c r="N8" s="11">
-        <v>57</v>
-      </c>
-      <c r="O8" s="11">
-        <v>85</v>
-      </c>
-      <c r="P8" s="11">
-        <v>85</v>
-      </c>
-      <c r="R8" s="11">
+      <c r="N8" s="6">
+        <v>57</v>
+      </c>
+      <c r="O8" s="6">
+        <v>85</v>
+      </c>
+      <c r="P8" s="6">
+        <v>85</v>
+      </c>
+      <c r="R8" s="6">
         <v>72</v>
       </c>
       <c r="S8" s="6">
@@ -1137,19 +1133,19 @@
       <c r="K9" s="6">
         <v>85</v>
       </c>
-      <c r="M9" s="11">
-        <v>56</v>
-      </c>
-      <c r="N9" s="11">
+      <c r="M9" s="6">
+        <v>56</v>
+      </c>
+      <c r="N9" s="6">
         <v>55</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="6">
         <v>113</v>
       </c>
-      <c r="P9" s="11">
-        <v>86</v>
-      </c>
-      <c r="R9" s="11">
+      <c r="P9" s="6">
+        <v>86</v>
+      </c>
+      <c r="R9" s="6">
         <v>72</v>
       </c>
       <c r="S9" s="6">
@@ -1204,19 +1200,19 @@
       <c r="K10" s="6">
         <v>82</v>
       </c>
-      <c r="M10" s="11">
-        <v>71</v>
-      </c>
-      <c r="N10" s="11">
-        <v>56</v>
-      </c>
-      <c r="O10" s="11">
-        <v>87</v>
-      </c>
-      <c r="P10" s="11">
-        <v>87</v>
-      </c>
-      <c r="R10" s="11">
+      <c r="M10" s="6">
+        <v>71</v>
+      </c>
+      <c r="N10" s="6">
+        <v>56</v>
+      </c>
+      <c r="O10" s="6">
+        <v>87</v>
+      </c>
+      <c r="P10" s="6">
+        <v>87</v>
+      </c>
+      <c r="R10" s="6">
         <v>72</v>
       </c>
       <c r="S10" s="6">
@@ -1271,19 +1267,19 @@
       <c r="K11" s="6">
         <v>83</v>
       </c>
-      <c r="M11" s="11">
-        <v>71</v>
-      </c>
-      <c r="N11" s="11">
-        <v>56</v>
-      </c>
-      <c r="O11" s="11">
+      <c r="M11" s="6">
+        <v>71</v>
+      </c>
+      <c r="N11" s="6">
+        <v>56</v>
+      </c>
+      <c r="O11" s="6">
         <v>93</v>
       </c>
-      <c r="P11" s="11">
-        <v>87</v>
-      </c>
-      <c r="R11" s="11">
+      <c r="P11" s="6">
+        <v>87</v>
+      </c>
+      <c r="R11" s="6">
         <v>71</v>
       </c>
       <c r="S11" s="6">
@@ -1338,19 +1334,19 @@
       <c r="K12" s="6">
         <v>83</v>
       </c>
-      <c r="M12" s="11">
-        <v>71</v>
-      </c>
-      <c r="N12" s="11">
-        <v>56</v>
-      </c>
-      <c r="O12" s="11">
-        <v>86</v>
-      </c>
-      <c r="P12" s="11">
-        <v>86</v>
-      </c>
-      <c r="R12" s="11">
+      <c r="M12" s="6">
+        <v>71</v>
+      </c>
+      <c r="N12" s="6">
+        <v>56</v>
+      </c>
+      <c r="O12" s="6">
+        <v>86</v>
+      </c>
+      <c r="P12" s="6">
+        <v>86</v>
+      </c>
+      <c r="R12" s="6">
         <v>73</v>
       </c>
       <c r="S12" s="6">
@@ -1405,19 +1401,19 @@
       <c r="K13" s="6">
         <v>83</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="6">
         <v>67</v>
       </c>
-      <c r="N13" s="11">
-        <v>57</v>
-      </c>
-      <c r="O13" s="11">
-        <v>86</v>
-      </c>
-      <c r="P13" s="11">
-        <v>88</v>
-      </c>
-      <c r="R13" s="11">
+      <c r="N13" s="6">
+        <v>57</v>
+      </c>
+      <c r="O13" s="6">
+        <v>86</v>
+      </c>
+      <c r="P13" s="6">
+        <v>88</v>
+      </c>
+      <c r="R13" s="6">
         <v>72</v>
       </c>
       <c r="S13" s="6">
@@ -1472,19 +1468,19 @@
       <c r="K14" s="6">
         <v>82</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="6">
         <v>70</v>
       </c>
-      <c r="N14" s="11">
-        <v>56</v>
-      </c>
-      <c r="O14" s="11">
-        <v>87</v>
-      </c>
-      <c r="P14" s="11">
-        <v>87</v>
-      </c>
-      <c r="R14" s="11">
+      <c r="N14" s="6">
+        <v>56</v>
+      </c>
+      <c r="O14" s="6">
+        <v>87</v>
+      </c>
+      <c r="P14" s="6">
+        <v>87</v>
+      </c>
+      <c r="R14" s="6">
         <v>72</v>
       </c>
       <c r="S14" s="6">
@@ -1539,19 +1535,19 @@
       <c r="K15" s="6">
         <v>83</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="6">
         <v>70</v>
       </c>
-      <c r="N15" s="11">
-        <v>56</v>
-      </c>
-      <c r="O15" s="11">
-        <v>86</v>
-      </c>
-      <c r="P15" s="11">
-        <v>87</v>
-      </c>
-      <c r="R15" s="11">
+      <c r="N15" s="6">
+        <v>56</v>
+      </c>
+      <c r="O15" s="6">
+        <v>86</v>
+      </c>
+      <c r="P15" s="6">
+        <v>87</v>
+      </c>
+      <c r="R15" s="6">
         <v>72</v>
       </c>
       <c r="S15" s="6">
@@ -1606,19 +1602,19 @@
       <c r="K16" s="6">
         <v>83</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="6">
         <v>65</v>
       </c>
-      <c r="N16" s="11">
-        <v>56</v>
-      </c>
-      <c r="O16" s="11">
-        <v>86</v>
-      </c>
-      <c r="P16" s="11">
-        <v>87</v>
-      </c>
-      <c r="R16" s="11">
+      <c r="N16" s="6">
+        <v>56</v>
+      </c>
+      <c r="O16" s="6">
+        <v>86</v>
+      </c>
+      <c r="P16" s="6">
+        <v>87</v>
+      </c>
+      <c r="R16" s="6">
         <v>69</v>
       </c>
       <c r="S16" s="6">
@@ -1673,19 +1669,19 @@
       <c r="K17" s="6">
         <v>83</v>
       </c>
-      <c r="M17" s="11">
-        <v>72</v>
-      </c>
-      <c r="N17" s="11">
-        <v>56</v>
-      </c>
-      <c r="O17" s="11">
-        <v>86</v>
-      </c>
-      <c r="P17" s="11">
+      <c r="M17" s="6">
+        <v>72</v>
+      </c>
+      <c r="N17" s="6">
+        <v>56</v>
+      </c>
+      <c r="O17" s="6">
+        <v>86</v>
+      </c>
+      <c r="P17" s="6">
         <v>90</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="6">
         <v>72</v>
       </c>
       <c r="S17" s="6">
@@ -1740,19 +1736,19 @@
       <c r="K18" s="6">
         <v>83</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="6">
         <v>68</v>
       </c>
-      <c r="N18" s="11">
-        <v>57</v>
-      </c>
-      <c r="O18" s="11">
-        <v>85</v>
-      </c>
-      <c r="P18" s="11">
-        <v>85</v>
-      </c>
-      <c r="R18" s="11">
+      <c r="N18" s="6">
+        <v>57</v>
+      </c>
+      <c r="O18" s="6">
+        <v>85</v>
+      </c>
+      <c r="P18" s="6">
+        <v>85</v>
+      </c>
+      <c r="R18" s="6">
         <v>73</v>
       </c>
       <c r="S18" s="6">
@@ -1807,19 +1803,19 @@
       <c r="K19" s="6">
         <v>104</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="6">
         <v>73</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="6">
         <v>55</v>
       </c>
-      <c r="O19" s="11">
-        <v>85</v>
-      </c>
-      <c r="P19" s="11">
-        <v>86</v>
-      </c>
-      <c r="R19" s="11">
+      <c r="O19" s="6">
+        <v>85</v>
+      </c>
+      <c r="P19" s="6">
+        <v>86</v>
+      </c>
+      <c r="R19" s="6">
         <v>74</v>
       </c>
       <c r="S19" s="6">
@@ -1874,19 +1870,19 @@
       <c r="K20" s="6">
         <v>82</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="6">
         <v>70</v>
       </c>
-      <c r="N20" s="11">
-        <v>57</v>
-      </c>
-      <c r="O20" s="11">
-        <v>85</v>
-      </c>
-      <c r="P20" s="11">
-        <v>86</v>
-      </c>
-      <c r="R20" s="11">
+      <c r="N20" s="6">
+        <v>57</v>
+      </c>
+      <c r="O20" s="6">
+        <v>85</v>
+      </c>
+      <c r="P20" s="6">
+        <v>86</v>
+      </c>
+      <c r="R20" s="6">
         <v>69</v>
       </c>
       <c r="S20" s="6">
@@ -1941,19 +1937,19 @@
       <c r="K21" s="6">
         <v>83</v>
       </c>
-      <c r="M21" s="11">
-        <v>71</v>
-      </c>
-      <c r="N21" s="11">
-        <v>56</v>
-      </c>
-      <c r="O21" s="11">
+      <c r="M21" s="6">
+        <v>71</v>
+      </c>
+      <c r="N21" s="6">
+        <v>56</v>
+      </c>
+      <c r="O21" s="6">
         <v>112</v>
       </c>
-      <c r="P21" s="11">
-        <v>85</v>
-      </c>
-      <c r="R21" s="11">
+      <c r="P21" s="6">
+        <v>85</v>
+      </c>
+      <c r="R21" s="6">
         <v>75</v>
       </c>
       <c r="S21" s="6">
@@ -1989,9 +1985,9 @@
         <v>85</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="5"/>
       <c r="I22" s="6">
         <v>66</v>
@@ -2002,11 +1998,11 @@
       <c r="K22" s="6">
         <v>83</v>
       </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="R22" s="11">
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="R22" s="6">
         <v>57</v>
       </c>
       <c r="S22" s="6">
@@ -2089,14 +2085,14 @@
         <f>AVERAGE(O3:O21)</f>
         <v>90.421052631578945</v>
       </c>
-      <c r="P23" s="13">
+      <c r="P23" s="11">
         <f>AVERAGE(P3:P21)</f>
         <v>86.631578947368425</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="6">
         <v>72</v>
       </c>
       <c r="S23" s="6">
@@ -2122,7 +2118,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="R24" s="11">
+      <c r="R24" s="6">
         <v>72</v>
       </c>
       <c r="S24" s="6">
@@ -2148,7 +2144,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="R25" s="11">
+      <c r="R25" s="6">
         <v>71</v>
       </c>
       <c r="S25" s="6">
@@ -2174,7 +2170,7 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="R26" s="11">
+      <c r="R26" s="6">
         <v>73</v>
       </c>
       <c r="S26" s="6">
@@ -2200,7 +2196,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="R27" s="11">
+      <c r="R27" s="6">
         <v>66</v>
       </c>
       <c r="S27" s="6">
@@ -2226,7 +2222,19 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="R28" s="11">
+      <c r="I28" s="9">
+        <f>AVERAGE(I23,E23,A23)</f>
+        <v>68.810317460317449</v>
+      </c>
+      <c r="J28" s="9">
+        <f>AVERAGE(J23,F23,B23)</f>
+        <v>56.664285714285711</v>
+      </c>
+      <c r="K28" s="9">
+        <f>AVERAGE(K23,G23,C23)</f>
+        <v>86.62222222222222</v>
+      </c>
+      <c r="R28" s="6">
         <v>72</v>
       </c>
       <c r="S28" s="6">
@@ -2252,8 +2260,7 @@
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="P29" s="8"/>
-      <c r="R29" s="11">
+      <c r="R29" s="6">
         <v>59</v>
       </c>
       <c r="S29" s="6">
@@ -2290,11 +2297,11 @@
         <f>AVERAGE(S2:S29)</f>
         <v>86.035714285714292</v>
       </c>
-      <c r="T30" s="13">
+      <c r="T30" s="11">
         <f>AVERAGE(T2:T29)</f>
         <v>86.964285714285708</v>
       </c>
-      <c r="U30" s="14">
+      <c r="U30" s="12">
         <f>AVERAGE(U2:U29)</f>
         <v>136.32142857142858</v>
       </c>
@@ -2371,7 +2378,7 @@
       </c>
     </row>
     <row r="35" spans="18:26" x14ac:dyDescent="0.2">
-      <c r="R35" s="17" t="s">
+      <c r="R35" s="15" t="s">
         <v>8</v>
       </c>
       <c r="W35" s="6">
@@ -2388,10 +2395,10 @@
       </c>
     </row>
     <row r="36" spans="18:26" x14ac:dyDescent="0.2">
-      <c r="R36" s="15" t="s">
+      <c r="R36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="S36" s="16">
+      <c r="S36" s="14">
         <f>AVERAGE(G2:G21,K2:K22,O3:O21,S2:S29,Y2:Y36)</f>
         <v>87.731707317073173</v>
       </c>
@@ -2409,10 +2416,10 @@
       </c>
     </row>
     <row r="37" spans="18:26" x14ac:dyDescent="0.2">
-      <c r="R37" s="15" t="s">
+      <c r="R37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="S37" s="16">
+      <c r="S37" s="14">
         <f>AVERAGE(P3:P21,T2:T29,Z2:Z36)</f>
         <v>87.792682926829272</v>
       </c>
@@ -2431,7 +2438,7 @@
         <f>AVERAGE(Y2:Y36)</f>
         <v>88.628571428571433</v>
       </c>
-      <c r="Z37" s="13">
+      <c r="Z37" s="11">
         <f>AVERAGE(Z2:Z36)</f>
         <v>89.085714285714289</v>
       </c>

</xml_diff>